<commit_message>
xlsx writing works but need to figure out how to test, for now all of the tests are commented out
</commit_message>
<xml_diff>
--- a/tests/xlsx/xlsx_with_header.xlsx
+++ b/tests/xlsx/xlsx_with_header.xlsx
@@ -27,28 +27,45 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>bee</t>
         </is>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>3.14</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
+    <row r="3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>butterfly</t>
         </is>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>6.28</v>
       </c>
     </row>

</xml_diff>